<commit_message>
Bug fixes, trainers and AI work
</commit_message>
<xml_diff>
--- a/stuff/xhenos story work.xlsx
+++ b/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\git\PokemonXhenos\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BD549C-2F1B-4B4B-AE93-E2D6B14EA595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE757816-1563-4C6C-8A69-2C1702CD2B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="400">
   <si>
     <t>Current</t>
   </si>
@@ -1233,6 +1233,9 @@
   </si>
   <si>
     <t>Deletor</t>
+  </si>
+  <si>
+    <t>Move Enc</t>
   </si>
 </sst>
 </file>
@@ -1613,7 +1616,7 @@
   <dimension ref="A1:AD154"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="AD34" sqref="AD34"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,6 +2265,9 @@
       <c r="L29" t="s">
         <v>392</v>
       </c>
+      <c r="M29" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">

</xml_diff>

<commit_message>
Work on settings, new sprite and got Extreme Mode lead selection done!
</commit_message>
<xml_diff>
--- a/stuff/xhenos story work.xlsx
+++ b/stuff/xhenos story work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\git\PokemonXhenos\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C96073F-56AC-480D-BB42-1BAC4548B5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0505CEFF-85EA-4B52-9A87-4835CC3C797B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="401">
   <si>
     <t>Current</t>
   </si>
@@ -1236,6 +1236,9 @@
   </si>
   <si>
     <t>Move Enc</t>
+  </si>
+  <si>
+    <t>Set Difficulty</t>
   </si>
 </sst>
 </file>
@@ -1616,7 +1619,7 @@
   <dimension ref="A1:AD154"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+      <selection activeCell="AC25" sqref="AC25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2014,6 +2017,9 @@
       <c r="AB25" t="s">
         <v>371</v>
       </c>
+      <c r="AC25" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">

</xml_diff>

<commit_message>
Bug fixes for the new update
</commit_message>
<xml_diff>
--- a/stuff/xhenos story work.xlsx
+++ b/stuff/xhenos story work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\git\PokemonXhenos\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0505CEFF-85EA-4B52-9A87-4835CC3C797B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B5168A-9781-498D-A03C-A86FFF118D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="402">
   <si>
     <t>Current</t>
   </si>
@@ -1239,6 +1239,9 @@
   </si>
   <si>
     <t>Set Difficulty</t>
+  </si>
+  <si>
+    <t>Rick Pad</t>
   </si>
 </sst>
 </file>
@@ -1619,7 +1622,7 @@
   <dimension ref="A1:AD154"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="AC25" sqref="AC25"/>
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,6 +2324,9 @@
       <c r="O30" t="s">
         <v>322</v>
       </c>
+      <c r="P30" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">

</xml_diff>

<commit_message>
2 new sprites and tons of changes during Italy 2-week trip!
</commit_message>
<xml_diff>
--- a/stuff/xhenos story work.xlsx
+++ b/stuff/xhenos story work.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\git\PokemonXhenos\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B5168A-9781-498D-A03C-A86FFF118D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB33463-B411-473B-96B2-803165345FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="407">
   <si>
     <t>Current</t>
   </si>
@@ -1242,6 +1242,21 @@
   </si>
   <si>
     <t>Rick Pad</t>
+  </si>
+  <si>
+    <t>Whiskeroar</t>
+  </si>
+  <si>
+    <t>Chlorie</t>
+  </si>
+  <si>
+    <t>Astrid</t>
+  </si>
+  <si>
+    <t>Arthra</t>
+  </si>
+  <si>
+    <t>Necrozma can be obtained once the player rematches the league and wins again, then after beating Ryder again he will have Necrozma call more of its kind by the ship in space</t>
   </si>
 </sst>
 </file>
@@ -1619,20 +1634,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
-  <dimension ref="A1:AD154"/>
+  <dimension ref="A1:AD155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" topLeftCell="B132" workbookViewId="0">
+      <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="165" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1643,7 +1658,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1654,7 +1669,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1662,7 +1677,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1670,7 +1685,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1681,7 +1696,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1692,7 +1707,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1700,7 +1715,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1708,7 +1723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1716,7 +1731,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1724,7 +1739,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1732,7 +1747,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1740,7 +1755,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1748,7 +1763,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1756,7 +1771,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1764,7 +1779,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1772,7 +1787,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1783,7 +1798,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1794,7 +1809,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1805,7 +1820,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1816,7 +1831,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1827,7 +1842,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1835,7 +1850,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1843,7 +1858,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1935,7 +1950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2024,7 +2039,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2116,7 +2131,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2181,7 +2196,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2237,7 +2252,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2278,7 +2293,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2328,7 +2343,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2402,7 +2417,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2494,7 +2509,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2553,7 +2568,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2569,8 +2584,20 @@
       <c r="E34" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>402</v>
+      </c>
+      <c r="L34" t="s">
+        <v>403</v>
+      </c>
+      <c r="M34" t="s">
+        <v>404</v>
+      </c>
+      <c r="N34" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2584,7 +2611,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2598,7 +2625,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2612,7 +2639,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2626,7 +2653,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2640,7 +2667,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2654,7 +2681,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2668,7 +2695,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2682,7 +2709,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2696,7 +2723,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2710,7 +2737,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2724,7 +2751,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2738,7 +2765,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2752,7 +2779,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2766,7 +2793,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2780,7 +2807,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2794,7 +2821,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2808,7 +2835,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2822,7 +2849,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2836,7 +2863,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2850,7 +2877,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2864,7 +2891,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2878,7 +2905,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2892,7 +2919,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2906,7 +2933,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -2920,7 +2947,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2934,7 +2961,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2942,7 +2969,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -2950,7 +2977,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2958,7 +2985,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -2966,7 +2993,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -2974,7 +3001,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -2982,7 +3009,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -2990,7 +3017,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -2998,7 +3025,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -3006,7 +3033,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -3014,7 +3041,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -3022,7 +3049,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -3030,7 +3057,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -3038,7 +3065,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -3046,7 +3073,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -3054,7 +3081,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -3062,7 +3089,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -3070,7 +3097,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -3078,7 +3105,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -3086,7 +3113,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -3094,7 +3121,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -3102,7 +3129,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -3110,17 +3137,17 @@
         <v>143</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>145</v>
       </c>
@@ -3128,349 +3155,354 @@
         <v>154</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B123" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B125" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B127" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B129" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B130" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B131" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B132" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B133" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B134" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B135" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B136" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B138" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B139" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B140" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B141" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B142" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B143" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B144" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B145" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B146" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B147" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B148" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B149" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B150" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B151" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B152" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B153" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B154" t="s">
         <v>391</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B155" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New sprite, Magic move animations and finished Bug move animations!
</commit_message>
<xml_diff>
--- a/stuff/xhenos story work.xlsx
+++ b/stuff/xhenos story work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\git\PokemonXhenos\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB33463-B411-473B-96B2-803165345FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6C0D95-6AB4-4F52-BE87-D25DEB2AFE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{271A13BE-4517-4656-AED4-3C6BEDDB1427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="408">
   <si>
     <t>Current</t>
   </si>
@@ -1257,6 +1257,9 @@
   </si>
   <si>
     <t>Necrozma can be obtained once the player rematches the league and wins again, then after beating Ryder again he will have Necrozma call more of its kind by the ship in space</t>
+  </si>
+  <si>
+    <t>Third Starter</t>
   </si>
 </sst>
 </file>
@@ -1636,18 +1639,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853A869-EFC3-49CB-8DC6-87B1B6715E26}">
   <dimension ref="A1:AD155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B132" workbookViewId="0">
-      <selection activeCell="B156" sqref="B156"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="165" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.44140625" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1658,7 +1661,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1669,7 +1672,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1685,7 +1688,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1696,7 +1699,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1707,7 +1710,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1715,7 +1718,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1723,7 +1726,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1731,7 +1734,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1739,7 +1742,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1747,7 +1750,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1755,7 +1758,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1763,7 +1766,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1779,7 +1782,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1787,7 +1790,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1798,7 +1801,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1809,7 +1812,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1820,7 +1823,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1831,7 +1834,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1842,7 +1845,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1850,7 +1853,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1858,7 +1861,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1950,7 +1953,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2039,7 +2042,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2131,7 +2134,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2196,7 +2199,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2252,7 +2255,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2293,7 +2296,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2343,7 +2346,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2417,7 +2420,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2509,7 +2512,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2567,8 +2570,11 @@
       <c r="S33" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T33" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2597,7 +2603,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2611,7 +2617,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2625,7 +2631,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2639,7 +2645,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2653,7 +2659,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2667,7 +2673,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2681,7 +2687,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2695,7 +2701,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2709,7 +2715,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2723,7 +2729,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2737,7 +2743,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2751,7 +2757,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2765,7 +2771,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2779,7 +2785,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2793,7 +2799,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2807,7 +2813,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2821,7 +2827,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2835,7 +2841,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2849,7 +2855,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2877,7 +2883,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2891,7 +2897,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2905,7 +2911,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2919,7 +2925,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2933,7 +2939,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -2947,7 +2953,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2961,7 +2967,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2969,7 +2975,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -2977,7 +2983,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2985,7 +2991,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -2993,7 +2999,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -3001,7 +3007,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -3009,7 +3015,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -3017,7 +3023,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -3025,7 +3031,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -3033,7 +3039,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -3041,7 +3047,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -3049,7 +3055,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -3057,7 +3063,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -3065,7 +3071,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -3073,7 +3079,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -3081,7 +3087,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -3089,7 +3095,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -3097,7 +3103,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -3105,7 +3111,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -3113,7 +3119,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -3121,7 +3127,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -3129,7 +3135,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -3137,17 +3143,17 @@
         <v>143</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>145</v>
       </c>
@@ -3155,352 +3161,352 @@
         <v>154</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>406</v>
       </c>

</xml_diff>